<commit_message>
Perbaiki keterangan format import
</commit_message>
<xml_diff>
--- a/assets/import/format_import_peserta_bantuan.xlsx
+++ b/assets/import/format_import_peserta_bantuan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\manurung\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F8A6A9-D6B5-4236-97A2-6BAE7782BCB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B91CD1-939C-4625-A111-045CC9F5F59F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>No. Peserta</t>
   </si>
@@ -79,16 +79,10 @@
     <t>Catatan:</t>
   </si>
   <si>
-    <t>1. Peserta Sasaran Penduduk adalah NIK</t>
-  </si>
-  <si>
-    <t>2. Peserta Sasaran Keluarga adalah No. KK</t>
-  </si>
-  <si>
-    <t>3. Peserta Sasaran RTM adalah No. RTM</t>
-  </si>
-  <si>
-    <t>4. Peserta Sasaran Kelompok adalah Kode Kelompok</t>
+    <t>1. Sesuaikan kolom peserta (A) berdasarkan sasaran : - penduduk = nik, - keluarga = no. kk, - rumah tangga = no. rtm, - kelompok = kode</t>
+  </si>
+  <si>
+    <t>2. Kolom Peserta (A) dan kolom NIK (C) wajib di isi, yang lain jika kosong data diambil dari data penduduk berdasarkan kolom NIK ©</t>
   </si>
 </sst>
 </file>
@@ -143,12 +137,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -560,23 +555,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>